<commit_message>
template manifest updated colors and formatting
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/manifest.xlsx
+++ b/resources/DatasetTemplate/manifest.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -79,33 +79,11 @@
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13.95"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="13.95"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="-webkit-standard"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,7 +93,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9DC3E6"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D08D"/>
+        <bgColor rgb="FF9DC3E6"/>
       </patternFill>
     </fill>
     <fill>
@@ -166,7 +150,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,24 +163,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -224,7 +200,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFA8D08D"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -272,63 +248,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" customFormat="false" ht="17.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="17.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
sds 3.0 manifest.xlsx first pass changes
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/manifest.xlsx
+++ b/resources/DatasetTemplate/manifest.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t xml:space="preserve">file type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data modality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also in dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also in dataset path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data dictionary path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity is transitive</t>
   </si>
   <si>
     <t xml:space="preserve">Additional Metadata</t>
@@ -155,23 +173,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,27 +265,139 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -280,13 +410,31 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
sds 3.0 freeze first row
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/manifest.xlsx
+++ b/resources/DatasetTemplate/manifest.xlsx
@@ -379,10 +379,12 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>

</xml_diff>